<commit_message>
QA Story- 46 Status: Completed. Message: Updated SettingTimeAttendanceSetupIndexPage.java,SettingTimeAttendanceSetupVerification.java,TestData.java
</commit_message>
<xml_diff>
--- a/Resource/DataConfiguration.xlsx
+++ b/Resource/DataConfiguration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Password</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>Baps@200</t>
+  </si>
+  <si>
+    <t>Url for signup Page</t>
+  </si>
+  <si>
+    <t>Url for Login Page</t>
+  </si>
+  <si>
+    <t>http://automation.zinghr.com/2015/Pages/Authentication/Login.aspx</t>
+  </si>
+  <si>
+    <t>http://automation.zinghr.com/2015/Pages/Authentication/Signup.aspx</t>
   </si>
 </sst>
 </file>
@@ -378,19 +390,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -400,8 +414,14 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -410,6 +430,12 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit: QA Story- 55 Status: Completed Message: Updated "TestData.java" And DataConfiguration.xlsx.
</commit_message>
<xml_diff>
--- a/Resource/DataConfiguration.xlsx
+++ b/Resource/DataConfiguration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Password</t>
   </si>
@@ -46,6 +46,133 @@
   </si>
   <si>
     <t>http://automation.zinghr.com/2015/Pages/Authentication/Signup.aspx</t>
+  </si>
+  <si>
+    <t>Employee Group</t>
+  </si>
+  <si>
+    <t>Leave Group</t>
+  </si>
+  <si>
+    <t>Calendar Group</t>
+  </si>
+  <si>
+    <t>Attendance Mode Group</t>
+  </si>
+  <si>
+    <t>Attendance Rule Group</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Salutation
+</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Last Name
+</t>
+  </si>
+  <si>
+    <t>Father Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Joining </t>
+  </si>
+  <si>
+    <t>Date of Confirmation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Address
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Country
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> State
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> City
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Postal Code
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PAN
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UAN
+</t>
+  </si>
+  <si>
+    <t>Mobile No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Official Email
+</t>
+  </si>
+  <si>
+    <t>Alternate Email</t>
+  </si>
+  <si>
+    <t>CardCode Mapping</t>
+  </si>
+  <si>
+    <t>Employment Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User Type
+</t>
+  </si>
+  <si>
+    <t>Attendance Mode 1</t>
+  </si>
+  <si>
+    <t>Attendance Mode 2</t>
+  </si>
+  <si>
+    <t>Attendance Mode 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Default Shift
+</t>
+  </si>
+  <si>
+    <t>Reporting Manager 1</t>
+  </si>
+  <si>
+    <t>Reporting Manager 2</t>
+  </si>
+  <si>
+    <t>Reporting Manager 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attendance Group </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Division </t>
   </si>
 </sst>
 </file>
@@ -92,9 +219,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -392,16 +522,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -448,13 +578,133 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:38" s="2" customFormat="1" ht="60">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Commit: QA Story- 58 Status: Completed Message: Updated "TestData.java" ; "EmployeeMasterIndexPage.java".
</commit_message>
<xml_diff>
--- a/Resource/DataConfiguration.xlsx
+++ b/Resource/DataConfiguration.xlsx
@@ -578,10 +578,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL1"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -700,6 +700,122 @@
       </c>
       <c r="AL1" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>13</v>
+      </c>
+      <c r="O2">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2">
+        <v>16</v>
+      </c>
+      <c r="R2">
+        <v>17</v>
+      </c>
+      <c r="S2">
+        <v>18</v>
+      </c>
+      <c r="T2">
+        <v>19</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
+      <c r="V2">
+        <v>21</v>
+      </c>
+      <c r="W2">
+        <v>22</v>
+      </c>
+      <c r="X2">
+        <v>23</v>
+      </c>
+      <c r="Y2">
+        <v>24</v>
+      </c>
+      <c r="Z2">
+        <v>25</v>
+      </c>
+      <c r="AA2">
+        <v>26</v>
+      </c>
+      <c r="AB2">
+        <v>27</v>
+      </c>
+      <c r="AC2">
+        <v>28</v>
+      </c>
+      <c r="AD2">
+        <v>29</v>
+      </c>
+      <c r="AE2">
+        <v>30</v>
+      </c>
+      <c r="AF2">
+        <v>31</v>
+      </c>
+      <c r="AG2">
+        <v>32</v>
+      </c>
+      <c r="AH2">
+        <v>33</v>
+      </c>
+      <c r="AI2">
+        <v>34</v>
+      </c>
+      <c r="AJ2">
+        <v>35</v>
+      </c>
+      <c r="AK2">
+        <v>36</v>
+      </c>
+      <c r="AL2">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>